<commit_message>
SW fixed T1 VCL listing
</commit_message>
<xml_diff>
--- a/docs/team/2019-zone4-team-schedule.xlsx
+++ b/docs/team/2019-zone4-team-schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shwor\Desktop\BCG-Zone-4\docs\team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{351FDFCF-2BF2-4EAF-BE70-CAD2BFEB4381}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B2C257-F310-4ABD-87B1-A8073AD5CF73}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18075" windowHeight="6510" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3750" yWindow="330" windowWidth="22350" windowHeight="15510" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Teams" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Team 2" sheetId="5" r:id="rId3"/>
     <sheet name="Team 3" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="49">
   <si>
     <t>Club</t>
   </si>
@@ -570,7 +570,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -614,15 +614,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -630,13 +627,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -656,26 +646,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1021,9 +1008,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A2:K12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1071,13 +1060,13 @@
       <c r="H2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="35">
+      <c r="I2" s="29">
         <v>43676</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="48">
+      <c r="K2" s="39">
         <v>43704</v>
       </c>
     </row>
@@ -1088,7 +1077,7 @@
       <c r="B3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="30" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="13" t="s">
@@ -1110,7 +1099,7 @@
       <c r="J3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1143,7 +1132,7 @@
         <v>23</v>
       </c>
       <c r="J4" s="20"/>
-      <c r="K4" s="21"/>
+      <c r="K4" s="18"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
@@ -1174,7 +1163,7 @@
         <v>15</v>
       </c>
       <c r="J5" s="20"/>
-      <c r="K5" s="21"/>
+      <c r="K5" s="18"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
@@ -1183,7 +1172,7 @@
       <c r="B6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="31" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="17" t="s">
@@ -1205,7 +1194,7 @@
         <v>30</v>
       </c>
       <c r="J6" s="20"/>
-      <c r="K6" s="21"/>
+      <c r="K6" s="18"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
@@ -1236,7 +1225,7 @@
       <c r="J7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="18" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1269,7 +1258,7 @@
         <v>6</v>
       </c>
       <c r="J8" s="20"/>
-      <c r="K8" s="21"/>
+      <c r="K8" s="18"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
@@ -1300,7 +1289,7 @@
         <v>13</v>
       </c>
       <c r="J9" s="20"/>
-      <c r="K9" s="21"/>
+      <c r="K9" s="18"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
@@ -1331,7 +1320,7 @@
         <v>9</v>
       </c>
       <c r="J10" s="20"/>
-      <c r="K10" s="21"/>
+      <c r="K10" s="18"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
@@ -1362,906 +1351,868 @@
         <v>5</v>
       </c>
       <c r="J11" s="20"/>
-      <c r="K11" s="21"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="K11" s="18"/>
+    </row>
+    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="40" t="s">
+      <c r="B12" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="40" t="s">
+      <c r="D12" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="40" t="s">
+      <c r="F12" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="I12" s="41" t="s">
+      <c r="H12" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="42"/>
-      <c r="K12" s="43"/>
-    </row>
-    <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="J12" s="37"/>
+      <c r="K12" s="23"/>
+    </row>
+    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5">
+        <v>43592</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="7">
+        <v>43620</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="9">
+        <v>43655</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="29">
+        <v>43676</v>
+      </c>
+      <c r="J15" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="39">
+        <v>43704</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="25" t="s">
+      <c r="F16" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="13"/>
+      <c r="I16" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="J13" s="44" t="s">
-        <v>3</v>
-      </c>
-      <c r="K13" s="26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="5">
-        <v>43592</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="7">
-        <v>43620</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" s="9">
-        <v>43655</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="I16" s="35">
-        <v>43676</v>
-      </c>
-      <c r="J16" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="K16" s="48">
-        <v>43704</v>
+      <c r="J16" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="14" t="s">
+      <c r="A17" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" s="18" t="s">
         <v>16</v>
-      </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="J17" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="K17" s="14" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="17"/>
+      <c r="I18" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" s="18" t="s">
         <v>17</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="I18" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="K18" s="18" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>3</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B19" s="17"/>
       <c r="C19" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="18" t="s">
+      <c r="H19" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" s="18" t="s">
         <v>33</v>
-      </c>
-      <c r="H19" s="17"/>
-      <c r="I19" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="K19" s="18" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="17"/>
+        <v>20</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>3</v>
+      </c>
       <c r="C20" s="18" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="F20" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H20" s="17" t="s">
         <v>3</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="K20" s="18" t="s">
-        <v>33</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="J20" s="17"/>
+      <c r="K20" s="18"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="18" t="s">
+      <c r="F21" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="18" t="s">
         <v>15</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="I21" s="18" t="s">
-        <v>18</v>
       </c>
       <c r="J21" s="17"/>
       <c r="K21" s="18"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="19" t="s">
+      <c r="F22" s="17"/>
+      <c r="G22" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="G22" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="I22" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="J22" s="17"/>
-      <c r="K22" s="18"/>
+      <c r="J22" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22" s="18" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="17"/>
+      <c r="I23" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K23" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="19" t="s">
+    </row>
+    <row r="24" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="I24" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" s="22"/>
+      <c r="K24" s="23"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="J25" s="38"/>
+    </row>
+    <row r="26" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5">
+        <v>43592</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="7">
+        <v>43620</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="9">
+        <v>43655</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="29">
+        <v>43676</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K27" s="39">
+        <v>43704</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18" t="s">
+      <c r="H28" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J28" s="17"/>
+      <c r="K28" s="18"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" s="17"/>
+      <c r="I29" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="I23" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="J23" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="K23" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="G24" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="H24" s="17"/>
-      <c r="I24" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="J24" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="K24" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="I25" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="J25" s="17"/>
-      <c r="K25" s="18"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="45"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="46"/>
-      <c r="K26" s="47"/>
-    </row>
-    <row r="27" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="5">
-        <v>43592</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28" s="7">
-        <v>43620</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G28" s="9">
-        <v>43655</v>
-      </c>
-      <c r="H28" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="I28" s="35">
-        <v>43676</v>
-      </c>
-      <c r="J28" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="K28" s="48">
-        <v>43704</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H29" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I29" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="J29" s="17"/>
-      <c r="K29" s="18"/>
+      <c r="J29" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="K29" s="18" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B30" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G30" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H30" s="17"/>
+        <v>17</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>3</v>
+      </c>
       <c r="I30" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="J30" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="K30" s="18" t="s">
-        <v>28</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="J30" s="17"/>
+      <c r="K30" s="18"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F31" s="17" t="s">
-        <v>3</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F31" s="17"/>
       <c r="G31" s="18" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I31" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="J31" s="17"/>
-      <c r="K31" s="18"/>
+        <v>37</v>
+      </c>
+      <c r="J31" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K31" s="18" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F32" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>7</v>
+      </c>
       <c r="G32" s="18" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="J32" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="K32" s="18" t="s">
-        <v>13</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="J32" s="17"/>
+      <c r="K32" s="18"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="H33" s="31" t="s">
-        <v>3</v>
+        <v>24</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>7</v>
       </c>
       <c r="I33" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J33" s="17"/>
       <c r="K33" s="18"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B34" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D34" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F34" s="17" t="s">
         <v>3</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="H34" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="17" t="s">
         <v>7</v>
       </c>
       <c r="I34" s="19" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="J34" s="17"/>
       <c r="K34" s="18"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F35" s="17" t="s">
         <v>3</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35" s="17" t="s">
         <v>7</v>
       </c>
       <c r="I35" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="J35" s="31"/>
+        <v>28</v>
+      </c>
+      <c r="J35" s="17"/>
       <c r="K35" s="18"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>3</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F36" s="17"/>
       <c r="G36" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="H36" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" s="17" t="s">
         <v>7</v>
       </c>
       <c r="I36" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="J36" s="31"/>
-      <c r="K36" s="18"/>
+        <v>36</v>
+      </c>
+      <c r="J36" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="K36" s="18" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>3</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B37" s="17"/>
       <c r="C37" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D37" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F37" s="17"/>
+        <v>26</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>3</v>
+      </c>
       <c r="G37" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="H37" s="31" t="s">
-        <v>7</v>
+        <v>25</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>3</v>
       </c>
       <c r="I37" s="19" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="J37" s="17" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K37" s="18" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F38" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="G38" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H38" s="31" t="s">
+      <c r="H38" s="17" t="s">
         <v>3</v>
       </c>
       <c r="I38" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J38" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="K38" s="18" t="s">
-        <v>23</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="J38" s="17"/>
+      <c r="K38" s="18"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>3</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B39" s="17"/>
       <c r="C39" s="18" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D39" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G39" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H39" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H39" s="17" t="s">
         <v>3</v>
       </c>
       <c r="I39" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="J39" s="31"/>
-      <c r="K39" s="18"/>
+        <v>16</v>
+      </c>
+      <c r="J39" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K39" s="18" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="18" t="s">
+      <c r="F40" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I40" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="17"/>
+      <c r="K40" s="18"/>
+    </row>
+    <row r="41" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41" s="22"/>
+      <c r="I41" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="G40" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H40" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="I40" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="J40" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="K40" s="18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E41" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F41" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="G41" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H41" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="I41" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="J41" s="31"/>
-      <c r="K41" s="18"/>
-    </row>
-    <row r="42" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B42" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E42" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="F42" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="G42" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="H42" s="23"/>
-      <c r="I42" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="J42" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="K42" s="24" t="s">
+      <c r="J41" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="K41" s="23" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.39370078740157483" bottom="0.39370078740157483" header="0.19685039370078741" footer="0.19685039370078741"/>
-  <pageSetup scale="76" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup scale="81" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>
@@ -2327,13 +2278,13 @@
       <c r="H2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="35">
+      <c r="I2" s="29">
         <v>43676</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="48">
+      <c r="K2" s="39">
         <v>43704</v>
       </c>
     </row>
@@ -2344,7 +2295,7 @@
       <c r="B3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="30" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="13" t="s">
@@ -2366,7 +2317,7 @@
       <c r="J3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2399,7 +2350,7 @@
         <v>23</v>
       </c>
       <c r="J4" s="20"/>
-      <c r="K4" s="21"/>
+      <c r="K4" s="18"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
@@ -2430,7 +2381,7 @@
         <v>15</v>
       </c>
       <c r="J5" s="20"/>
-      <c r="K5" s="21"/>
+      <c r="K5" s="18"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
@@ -2439,7 +2390,7 @@
       <c r="B6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="31" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="17" t="s">
@@ -2461,7 +2412,7 @@
         <v>30</v>
       </c>
       <c r="J6" s="20"/>
-      <c r="K6" s="21"/>
+      <c r="K6" s="18"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
@@ -2492,7 +2443,7 @@
       <c r="J7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="18" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2525,7 +2476,7 @@
         <v>6</v>
       </c>
       <c r="J8" s="20"/>
-      <c r="K8" s="21"/>
+      <c r="K8" s="18"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
@@ -2556,7 +2507,7 @@
         <v>13</v>
       </c>
       <c r="J9" s="20"/>
-      <c r="K9" s="21"/>
+      <c r="K9" s="18"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
@@ -2587,7 +2538,7 @@
         <v>9</v>
       </c>
       <c r="J10" s="20"/>
-      <c r="K10" s="21"/>
+      <c r="K10" s="18"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
@@ -2618,80 +2569,80 @@
         <v>5</v>
       </c>
       <c r="J11" s="20"/>
-      <c r="K11" s="21"/>
+      <c r="K11" s="18"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="40" t="s">
+      <c r="B12" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="40" t="s">
+      <c r="D12" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="40" t="s">
+      <c r="F12" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="I12" s="41" t="s">
+      <c r="H12" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="42"/>
-      <c r="K12" s="43"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="34"/>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="34" t="s">
+      <c r="B13" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="24" t="s">
+      <c r="D13" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="24" t="s">
+      <c r="F13" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="25" t="s">
+      <c r="H13" s="22"/>
+      <c r="I13" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="J13" s="44" t="s">
-        <v>3</v>
-      </c>
-      <c r="K13" s="26" t="s">
+      <c r="J13" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="23" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="49" t="s">
+      <c r="D15" s="40" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2731,7 +2682,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2745,7 +2696,7 @@
       <c r="C2" s="5">
         <v>43592</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="25" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="7">
@@ -2760,13 +2711,13 @@
       <c r="H2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="35">
+      <c r="I2" s="29">
         <v>43676</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="48">
+      <c r="K2" s="39">
         <v>43704</v>
       </c>
     </row>
@@ -3062,26 +3013,21 @@
       <c r="K11" s="18"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="47"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="J12" s="38"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="50" t="s">
+      <c r="D13" s="41" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3150,13 +3096,13 @@
       <c r="H2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="35">
+      <c r="I2" s="29">
         <v>43676</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="48">
+      <c r="K2" s="39">
         <v>43704</v>
       </c>
     </row>
@@ -3173,7 +3119,7 @@
       <c r="D3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="27" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="13" t="s">
@@ -3310,7 +3256,7 @@
       <c r="G7" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="31" t="s">
+      <c r="H7" s="17" t="s">
         <v>3</v>
       </c>
       <c r="I7" s="19" t="s">
@@ -3341,7 +3287,7 @@
       <c r="G8" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="31" t="s">
+      <c r="H8" s="17" t="s">
         <v>7</v>
       </c>
       <c r="I8" s="19" t="s">
@@ -3372,13 +3318,13 @@
       <c r="G9" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="H9" s="17" t="s">
         <v>7</v>
       </c>
       <c r="I9" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="31"/>
+      <c r="J9" s="17"/>
       <c r="K9" s="18"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -3403,13 +3349,13 @@
       <c r="G10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="17" t="s">
         <v>7</v>
       </c>
       <c r="I10" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="31"/>
+      <c r="J10" s="17"/>
       <c r="K10" s="18"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3432,7 +3378,7 @@
       <c r="G11" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="17" t="s">
         <v>7</v>
       </c>
       <c r="I11" s="19" t="s">
@@ -3465,13 +3411,13 @@
       <c r="G12" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="31" t="s">
+      <c r="H12" s="17" t="s">
         <v>3</v>
       </c>
       <c r="I12" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="31" t="s">
+      <c r="J12" s="17" t="s">
         <v>7</v>
       </c>
       <c r="K12" s="18" t="s">
@@ -3500,13 +3446,13 @@
       <c r="G13" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="31" t="s">
+      <c r="H13" s="17" t="s">
         <v>3</v>
       </c>
       <c r="I13" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="31"/>
+      <c r="J13" s="17"/>
       <c r="K13" s="18"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3529,13 +3475,13 @@
       <c r="G14" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="31" t="s">
+      <c r="H14" s="17" t="s">
         <v>3</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="31" t="s">
+      <c r="J14" s="17" t="s">
         <v>7</v>
       </c>
       <c r="K14" s="18" t="s">
@@ -3564,45 +3510,45 @@
       <c r="G15" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="31" t="s">
+      <c r="H15" s="17" t="s">
         <v>7</v>
       </c>
       <c r="I15" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="31"/>
+      <c r="J15" s="17"/>
       <c r="K15" s="18"/>
     </row>
     <row r="16" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="24" t="s">
+      <c r="B16" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="24" t="s">
+      <c r="D16" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="24" t="s">
+      <c r="F16" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="23"/>
-      <c r="I16" s="25" t="s">
+      <c r="H16" s="22"/>
+      <c r="I16" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="K16" s="24" t="s">
+      <c r="J16" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" s="23" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3612,13 +3558,13 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="50" t="s">
+      <c r="D19" s="41" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>